<commit_message>
Converted program to use dictionaries. Should make addition of new features streamlined.
</commit_message>
<xml_diff>
--- a/TheKesselRun/Data/NH3Data.xlsx
+++ b/TheKesselRun/Data/NH3Data.xlsx
@@ -146,24 +146,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="54">
   <si>
-    <t>Metal 1</t>
-  </si>
-  <si>
-    <t>M1 Wt %</t>
-  </si>
-  <si>
-    <t>Metal 2</t>
-  </si>
-  <si>
-    <t>M2 Wt %</t>
-  </si>
-  <si>
-    <t>Metal 3</t>
-  </si>
-  <si>
-    <t>M3 Wt %</t>
-  </si>
-  <si>
     <t>T250</t>
   </si>
   <si>
@@ -306,6 +288,24 @@
   </si>
   <si>
     <t>Ammonia Concentration</t>
+  </si>
+  <si>
+    <t>Element_1</t>
+  </si>
+  <si>
+    <t>Loading_1</t>
+  </si>
+  <si>
+    <t>Element_2</t>
+  </si>
+  <si>
+    <t>Loading_2</t>
+  </si>
+  <si>
+    <t>Element_3</t>
+  </si>
+  <si>
+    <t>Loading_3</t>
   </si>
 </sst>
 </file>
@@ -744,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="P61" sqref="P2:P61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,72 +757,72 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="I1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="L1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>10</v>
-      </c>
       <c r="M1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="P1" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C2" s="6">
         <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E2" s="7">
         <v>1</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G2" s="8">
         <v>12</v>
@@ -857,22 +857,22 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C3" s="6">
         <v>2</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E3" s="7">
         <v>2</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G3" s="8">
         <v>12</v>
@@ -907,22 +907,22 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C4" s="6">
         <v>1</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E4" s="7">
         <v>3</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G4" s="8">
         <v>12</v>
@@ -957,22 +957,22 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C5" s="6">
         <v>4</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E5" s="7">
         <v>0</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G5" s="8">
         <v>0</v>
@@ -1007,22 +1007,22 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C6" s="6">
         <v>3</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E6" s="7">
         <v>1</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G6" s="8">
         <v>12</v>
@@ -1057,22 +1057,22 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C7" s="6">
         <v>2</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E7" s="7">
         <v>2</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G7" s="8">
         <v>12</v>
@@ -1107,22 +1107,22 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C8" s="6">
         <v>1</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E8" s="7">
         <v>3</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G8" s="8">
         <v>12</v>
@@ -1157,22 +1157,22 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C9" s="6">
         <v>3</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E9" s="7">
         <v>1</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G9" s="8">
         <v>12</v>
@@ -1207,22 +1207,22 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C10" s="6">
         <v>2</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E10" s="7">
         <v>2</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G10" s="8">
         <v>12</v>
@@ -1257,22 +1257,22 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C11" s="6">
         <v>1</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E11" s="7">
         <v>3</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G11" s="8">
         <v>12</v>
@@ -1307,22 +1307,22 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C12" s="6">
         <v>12</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E12" s="7">
         <v>0</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G12" s="8">
         <v>0</v>
@@ -1357,22 +1357,22 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C13" s="6">
         <v>3</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E13" s="7">
         <v>1</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G13" s="8">
         <v>12</v>
@@ -1410,19 +1410,19 @@
         <v>38</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C14" s="6">
         <v>2</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E14" s="7">
         <v>2</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G14" s="8">
         <v>12</v>
@@ -1460,19 +1460,19 @@
         <v>39</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C15" s="6">
         <v>1</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E15" s="7">
         <v>3</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G15" s="8">
         <v>12</v>
@@ -1510,19 +1510,19 @@
         <v>40</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C16" s="6">
         <v>3</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E16" s="7">
         <v>1</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G16" s="8">
         <v>12</v>
@@ -1560,19 +1560,19 @@
         <v>45</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C17" s="6">
         <v>1</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E17" s="7">
         <v>3</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G17" s="8">
         <v>12</v>
@@ -1610,19 +1610,19 @@
         <v>49</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C18" s="6">
         <v>3</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E18" s="7">
         <v>1</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G18" s="8">
         <v>12</v>
@@ -1660,19 +1660,19 @@
         <v>50</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C19" s="6">
         <v>2</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E19" s="7">
         <v>2</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G19" s="8">
         <v>12</v>
@@ -1710,19 +1710,19 @@
         <v>51</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C20" s="6">
         <v>1</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E20" s="7">
         <v>3</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G20" s="8">
         <v>12</v>
@@ -1760,19 +1760,19 @@
         <v>55</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C21" s="6">
         <v>3</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E21" s="7">
         <v>1</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G21" s="8">
         <v>12</v>
@@ -1810,19 +1810,19 @@
         <v>56</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C22" s="6">
         <v>2</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E22" s="7">
         <v>2</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G22" s="8">
         <v>12</v>
@@ -1860,19 +1860,19 @@
         <v>20</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C23" s="6">
         <v>4</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E23" s="7">
         <v>0</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G23" s="8">
         <v>12</v>
@@ -1910,19 +1910,19 @@
         <v>21</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C24" s="6">
         <v>4</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E24" s="7">
         <v>0</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G24" s="8">
         <v>12</v>
@@ -1960,19 +1960,19 @@
         <v>22</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C25" s="6">
         <v>4</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E25" s="7">
         <v>0</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G25" s="8">
         <v>12</v>
@@ -2010,19 +2010,19 @@
         <v>21</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C26" s="6">
         <v>4</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E26" s="7">
         <v>0</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G26" s="8">
         <v>12</v>
@@ -2052,19 +2052,19 @@
         <v>24</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C27" s="6">
         <v>4</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E27" s="7">
         <v>0</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G27" s="8">
         <v>12</v>
@@ -2102,19 +2102,19 @@
         <v>43</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C28" s="6">
         <v>3</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E28" s="7">
         <v>1</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G28" s="8">
         <v>12</v>
@@ -2152,19 +2152,19 @@
         <v>44</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C29" s="6">
         <v>2</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E29" s="7">
         <v>2</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G29" s="8">
         <v>12</v>
@@ -2202,19 +2202,19 @@
         <v>25</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C30" s="6">
         <v>4</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E30" s="7">
         <v>0</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G30" s="8">
         <v>0</v>
@@ -2252,19 +2252,19 @@
         <v>31</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C31" s="6">
         <v>1</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E31" s="7">
         <v>3</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G31" s="8">
         <v>12</v>
@@ -2302,19 +2302,19 @@
         <v>33</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C32" s="6">
         <v>3</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E32" s="7">
         <v>1</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G32" s="8">
         <v>12</v>
@@ -2352,19 +2352,19 @@
         <v>40</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C33" s="6">
         <v>3</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E33" s="7">
         <v>1</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G33" s="8">
         <v>12</v>
@@ -2402,19 +2402,19 @@
         <v>41</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C34" s="6">
         <v>2</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E34" s="7">
         <v>2</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G34" s="8">
         <v>12</v>
@@ -2452,19 +2452,19 @@
         <v>42</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C35" s="6">
         <v>1</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E35" s="7">
         <v>3</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G35" s="8">
         <v>12</v>
@@ -2502,19 +2502,19 @@
         <v>112</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C36" s="6">
         <v>2</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E36" s="7">
         <v>2</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G36" s="8">
         <v>0</v>
@@ -2552,19 +2552,19 @@
         <v>113</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C37" s="6">
         <v>2</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E37" s="7">
         <v>2</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G37" s="8">
         <v>0</v>
@@ -2602,19 +2602,19 @@
         <v>114</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C38" s="6">
         <v>2</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E38" s="7">
         <v>2</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G38" s="8">
         <v>0</v>
@@ -2652,19 +2652,19 @@
         <v>115</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C39" s="6">
         <v>2</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E39" s="7">
         <v>2</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G39" s="8">
         <v>0</v>
@@ -2702,19 +2702,19 @@
         <v>116</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C40" s="6">
         <v>2</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E40" s="7">
         <v>2</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G40" s="8">
         <v>0</v>
@@ -2752,19 +2752,19 @@
         <v>117</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C41" s="6">
         <v>2</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E41" s="7">
         <v>2</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G41" s="8">
         <v>0</v>
@@ -2802,19 +2802,19 @@
         <v>118</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C42" s="6">
         <v>2</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E42" s="7">
         <v>2</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G42" s="8">
         <v>0</v>
@@ -2852,19 +2852,19 @@
         <v>119</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C43" s="6">
         <v>2</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E43" s="7">
         <v>2</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G43" s="8">
         <v>0</v>
@@ -2902,19 +2902,19 @@
         <v>57</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C44" s="6">
         <v>1</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E44" s="7">
         <v>3</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G44" s="8">
         <v>12</v>
@@ -2952,19 +2952,19 @@
         <v>106</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C45" s="6">
         <v>3</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E45" s="7">
         <v>1</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G45" s="8">
         <v>12</v>
@@ -3002,19 +3002,19 @@
         <v>107</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C46" s="6">
         <v>2</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E46" s="7">
         <v>2</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G46" s="8">
         <v>12</v>
@@ -3052,19 +3052,19 @@
         <v>108</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C47" s="6">
         <v>1</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E47" s="7">
         <v>3</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G47" s="8">
         <v>12</v>
@@ -3102,19 +3102,19 @@
         <v>58</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C48" s="6">
         <v>3</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E48" s="7">
         <v>1</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G48" s="8">
         <v>12</v>
@@ -3152,19 +3152,19 @@
         <v>59</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C49" s="6">
         <v>2</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E49" s="7">
         <v>2</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G49" s="8">
         <v>12</v>
@@ -3202,19 +3202,19 @@
         <v>60</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C50" s="6">
         <v>1</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E50" s="7">
         <v>3</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G50" s="8">
         <v>12</v>
@@ -3252,19 +3252,19 @@
         <v>120</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C51" s="6">
         <v>2</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E51" s="7">
         <v>2</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G51" s="8">
         <v>0</v>
@@ -3302,19 +3302,19 @@
         <v>121</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C52" s="6">
         <v>2</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E52" s="7">
         <v>2</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G52" s="8">
         <v>0</v>
@@ -3352,19 +3352,19 @@
         <v>122</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C53" s="6">
         <v>2</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E53" s="7">
         <v>2</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G53" s="8">
         <v>0</v>
@@ -3402,19 +3402,19 @@
         <v>123</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C54" s="6">
         <v>2</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E54" s="7">
         <v>2</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G54" s="8">
         <v>0</v>
@@ -3452,19 +3452,19 @@
         <v>124</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C55" s="6">
         <v>4</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E55" s="7">
         <v>0</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G55" s="8">
         <v>12</v>
@@ -3502,19 +3502,19 @@
         <v>125</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C56" s="6">
         <v>4</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E56" s="7">
         <v>0</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G56" s="8">
         <v>0</v>
@@ -3552,19 +3552,19 @@
         <v>126</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C57" s="6">
         <v>1</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E57" s="7">
         <v>3</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G57" s="8">
         <v>0</v>
@@ -3602,19 +3602,19 @@
         <v>61</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C58" s="6">
         <v>3</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E58" s="7">
         <v>1</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G58" s="8">
         <v>12</v>
@@ -3652,19 +3652,19 @@
         <v>62</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C59" s="6">
         <v>2</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E59" s="7">
         <v>2</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G59" s="8">
         <v>12</v>
@@ -3702,19 +3702,19 @@
         <v>63</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C60" s="6">
         <v>1</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E60" s="7">
         <v>3</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G60" s="8">
         <v>12</v>
@@ -3752,19 +3752,19 @@
         <v>64</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C61" s="6">
         <v>3</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E61" s="7">
         <v>1</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G61" s="8">
         <v>12</v>
@@ -3803,7 +3803,7 @@
         <v>14</v>
       </c>
       <c r="N62" s="12" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="O62" s="12" t="e">
         <v>#VALUE!</v>
@@ -3815,7 +3815,7 @@
         <v>15</v>
       </c>
       <c r="N63" s="12" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="O63" s="12" t="e">
         <v>#VALUE!</v>
@@ -3826,7 +3826,7 @@
         <v>13</v>
       </c>
       <c r="N64" s="12" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="O64" s="12">
         <v>2548.2590564236548</v>

</xml_diff>

<commit_message>
Rearranging Code Added Minor Functions Combined functions for readability
</commit_message>
<xml_diff>
--- a/TheKesselRun/Data/NH3Data.xlsx
+++ b/TheKesselRun/Data/NH3Data.xlsx
@@ -19,7 +19,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A23" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -43,7 +43,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A24" authorId="0" shapeId="0">
+    <comment ref="A3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -67,7 +67,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="A25" authorId="0" shapeId="0">
+    <comment ref="A4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+RuK 6mL washed</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -91,31 +115,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A26" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-RuK 6mL washed</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A27" authorId="0" shapeId="0">
+    <comment ref="A6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -745,11 +745,15 @@
   <dimension ref="A1:R141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H17" sqref="H17:L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="23" bestFit="1" customWidth="1"/>
@@ -806,158 +810,148 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>12</v>
+      <c r="A2" s="10">
+        <v>20</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="6">
+        <v>4</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="8">
+        <v>12</v>
+      </c>
+      <c r="H2" s="15">
+        <v>8.8448772441250378E-2</v>
+      </c>
+      <c r="I2" s="15">
+        <v>0.36900303806969204</v>
+      </c>
+      <c r="J2" s="15">
+        <v>0.92378999312359533</v>
+      </c>
+      <c r="K2" s="15">
+        <v>0.93264450938087895</v>
+      </c>
+      <c r="L2" s="15">
+        <v>0.96509621425660008</v>
+      </c>
+      <c r="M2" s="12">
+        <v>0</v>
+      </c>
+      <c r="N2" s="14">
+        <v>43133</v>
+      </c>
+      <c r="O2" s="12">
+        <v>2057.9500000000003</v>
+      </c>
+      <c r="P2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>21</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="6">
+        <v>4</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="8">
+        <v>12</v>
+      </c>
+      <c r="H3" s="15">
+        <v>0.19209965864266101</v>
+      </c>
+      <c r="I3" s="15">
+        <v>0.48492784095629798</v>
+      </c>
+      <c r="J3" s="15">
+        <v>0.9579800523816504</v>
+      </c>
+      <c r="K3" s="15">
+        <v>1.0091528910794141</v>
+      </c>
+      <c r="L3" s="15">
+        <v>1.0011138713772796</v>
+      </c>
+      <c r="M3" s="12">
+        <v>1</v>
+      </c>
+      <c r="N3" s="14">
+        <v>43133</v>
+      </c>
+      <c r="O3" s="12">
+        <v>2162.7227722772277</v>
+      </c>
+      <c r="P3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>21</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="6">
+        <v>4</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="8">
+        <v>12</v>
+      </c>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="12">
         <v>3</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="7">
-        <v>1</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="8">
-        <v>12</v>
-      </c>
-      <c r="H2" s="16">
-        <v>9.4557951106624946E-2</v>
-      </c>
-      <c r="I2" s="16">
-        <v>0.1516853288512657</v>
-      </c>
-      <c r="J2" s="16">
-        <v>0.42895787388935297</v>
-      </c>
-      <c r="K2" s="16">
-        <v>0.95785891995849859</v>
-      </c>
-      <c r="L2" s="16">
-        <v>0.98499562083574521</v>
-      </c>
-      <c r="M2" s="11">
-        <v>0</v>
-      </c>
-      <c r="N2" s="14">
-        <v>43125</v>
-      </c>
-      <c r="O2" s="12">
-        <v>2092.9104477611941</v>
-      </c>
-      <c r="P2">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="6">
-        <v>2</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="7">
-        <v>2</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="8">
-        <v>12</v>
-      </c>
-      <c r="H3" s="16">
-        <v>0.1195358705393363</v>
-      </c>
-      <c r="I3" s="16">
-        <v>0.13020674324129303</v>
-      </c>
-      <c r="J3" s="16">
-        <v>0.26005971336636069</v>
-      </c>
-      <c r="K3" s="16">
-        <v>0.61923951149020506</v>
-      </c>
-      <c r="L3" s="16">
-        <v>0.9877742331075684</v>
-      </c>
-      <c r="M3" s="11">
-        <v>1</v>
-      </c>
-      <c r="N3" s="14">
-        <v>43125</v>
-      </c>
-      <c r="O3" s="12">
-        <v>2176.4500000000003</v>
-      </c>
-      <c r="P3">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="6">
-        <v>1</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="7">
-        <v>3</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="8">
-        <v>12</v>
-      </c>
-      <c r="H4" s="16">
-        <v>0.19121111974535329</v>
-      </c>
-      <c r="I4" s="16">
-        <v>0.20612223570706134</v>
-      </c>
-      <c r="J4" s="16">
-        <v>0.27641542918024836</v>
-      </c>
-      <c r="K4" s="16">
-        <v>0.49135286954756102</v>
-      </c>
-      <c r="L4" s="16">
-        <v>0.86123370634274699</v>
-      </c>
-      <c r="M4" s="11">
-        <v>3</v>
-      </c>
       <c r="N4" s="14">
-        <v>43125</v>
+        <v>43133</v>
       </c>
       <c r="O4" s="12">
-        <v>2354.2000000000003</v>
+        <v>2214.6844660194179</v>
       </c>
       <c r="P4">
         <v>0.01</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>15</v>
+      <c r="A5" s="10">
+        <v>22</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>5</v>
@@ -972,142 +966,142 @@
         <v>0</v>
       </c>
       <c r="F5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="8">
+        <v>12</v>
+      </c>
+      <c r="H5" s="15">
+        <v>0.11327374860787404</v>
+      </c>
+      <c r="I5" s="15">
+        <v>0.34762514691913898</v>
+      </c>
+      <c r="J5" s="15">
+        <v>0.8354540499474985</v>
+      </c>
+      <c r="K5" s="15">
+        <v>0.97479817949538916</v>
+      </c>
+      <c r="L5" s="15">
+        <v>0.96599747056483165</v>
+      </c>
+      <c r="M5" s="12">
+        <v>2</v>
+      </c>
+      <c r="N5" s="14">
+        <v>43133</v>
+      </c>
+      <c r="O5" s="12">
+        <v>2787.5</v>
+      </c>
+      <c r="P5">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>24</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6">
+        <v>4</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="8">
+        <v>12</v>
+      </c>
+      <c r="H6" s="15">
+        <v>0.32913075782129203</v>
+      </c>
+      <c r="I6" s="15">
+        <v>0.40436473524431332</v>
+      </c>
+      <c r="J6" s="15">
+        <v>0.62151391999376759</v>
+      </c>
+      <c r="K6" s="15">
+        <v>0.99099383606947011</v>
+      </c>
+      <c r="L6" s="15">
+        <v>0.97395274989101532</v>
+      </c>
+      <c r="M6" s="12">
+        <v>4</v>
+      </c>
+      <c r="N6" s="14">
+        <v>43133</v>
+      </c>
+      <c r="O6" s="12">
+        <v>1937.4849246231156</v>
+      </c>
+      <c r="P6">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>25</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="6">
+        <v>4</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G7" s="8">
         <v>0</v>
       </c>
-      <c r="H5" s="16">
-        <v>0.26671957824088333</v>
-      </c>
-      <c r="I5" s="16">
-        <v>0.4611335403017584</v>
-      </c>
-      <c r="J5" s="16">
-        <v>0.94082183810715747</v>
-      </c>
-      <c r="K5" s="16">
-        <v>1</v>
-      </c>
-      <c r="L5" s="16">
-        <v>1</v>
-      </c>
-      <c r="M5" s="11">
-        <v>4</v>
-      </c>
-      <c r="N5" s="14">
-        <v>43125</v>
-      </c>
-      <c r="O5" s="12">
-        <v>1925.625</v>
-      </c>
-      <c r="P5">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="6">
-        <v>3</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="7">
-        <v>1</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="8">
-        <v>12</v>
-      </c>
-      <c r="H6" s="16">
-        <v>0.50969447771133602</v>
-      </c>
-      <c r="I6" s="16">
-        <v>0.94519530746047431</v>
-      </c>
-      <c r="J6" s="16">
-        <v>0.96635511610319114</v>
-      </c>
-      <c r="K6" s="16">
-        <v>0.95752529870093561</v>
-      </c>
-      <c r="L6" s="16">
-        <v>0.9576437682443496</v>
-      </c>
-      <c r="M6" s="11">
-        <v>5</v>
-      </c>
-      <c r="N6" s="14">
-        <v>43125</v>
-      </c>
-      <c r="O6" s="12">
-        <v>1825.8875</v>
-      </c>
-      <c r="P6">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="6">
-        <v>2</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="7">
-        <v>2</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="8">
-        <v>12</v>
-      </c>
-      <c r="H7" s="16">
-        <v>0.46819270517182704</v>
-      </c>
-      <c r="I7" s="16">
-        <v>0.89407361672624663</v>
-      </c>
-      <c r="J7" s="16">
-        <v>1</v>
-      </c>
-      <c r="K7" s="16">
-        <v>1</v>
-      </c>
-      <c r="L7" s="16">
-        <v>1</v>
-      </c>
-      <c r="M7" s="11">
-        <v>6</v>
+      <c r="H7" s="15">
+        <v>0.24675021175493536</v>
+      </c>
+      <c r="I7" s="15">
+        <v>0.28733107150260734</v>
+      </c>
+      <c r="J7" s="15">
+        <v>0.49512127230716052</v>
+      </c>
+      <c r="K7" s="15">
+        <v>0.8486639983684201</v>
+      </c>
+      <c r="L7" s="15">
+        <v>0.93491784964297076</v>
+      </c>
+      <c r="M7" s="12">
+        <v>9</v>
       </c>
       <c r="N7" s="14">
-        <v>43125</v>
+        <v>43133</v>
       </c>
       <c r="O7" s="12">
-        <v>2366.0301507537688</v>
+        <v>1975</v>
       </c>
       <c r="P7">
         <v>0.01</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>18</v>
+      <c r="A8" s="10">
+        <v>31</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>5</v>
@@ -1127,37 +1121,37 @@
       <c r="G8" s="8">
         <v>12</v>
       </c>
-      <c r="H8" s="16">
-        <v>0.39237353123262569</v>
-      </c>
-      <c r="I8" s="16">
-        <v>0.84077737958456444</v>
-      </c>
-      <c r="J8" s="16">
-        <v>1</v>
-      </c>
-      <c r="K8" s="16">
-        <v>1</v>
-      </c>
-      <c r="L8" s="16">
-        <v>1</v>
-      </c>
-      <c r="M8" s="11">
-        <v>7</v>
+      <c r="H8" s="15">
+        <v>0.20494025535697469</v>
+      </c>
+      <c r="I8" s="15">
+        <v>0.32319328315160306</v>
+      </c>
+      <c r="J8" s="15">
+        <v>0.74540804107981595</v>
+      </c>
+      <c r="K8" s="15">
+        <v>0.95552327266352266</v>
+      </c>
+      <c r="L8" s="15">
+        <v>0.97407546577591397</v>
+      </c>
+      <c r="M8" s="12">
+        <v>10</v>
       </c>
       <c r="N8" s="14">
-        <v>43125</v>
+        <v>43133</v>
       </c>
       <c r="O8" s="12">
-        <v>1986.85</v>
+        <v>2008.575</v>
       </c>
       <c r="P8">
         <v>0.01</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>19</v>
+      <c r="A9" s="10">
+        <v>33</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>5</v>
@@ -1177,37 +1171,37 @@
       <c r="G9" s="8">
         <v>12</v>
       </c>
-      <c r="H9" s="16">
-        <v>0.53459733253159325</v>
-      </c>
-      <c r="I9" s="16">
-        <v>0.97504215970422059</v>
-      </c>
-      <c r="J9" s="16">
-        <v>1</v>
-      </c>
-      <c r="K9" s="16">
-        <v>1</v>
-      </c>
-      <c r="L9" s="16">
-        <v>1</v>
-      </c>
-      <c r="M9" s="11">
-        <v>9</v>
+      <c r="H9" s="15">
+        <v>0.38772385066941001</v>
+      </c>
+      <c r="I9" s="15">
+        <v>0.5049664106522217</v>
+      </c>
+      <c r="J9" s="15">
+        <v>0.81580047533790245</v>
+      </c>
+      <c r="K9" s="15">
+        <v>0.98184797965604254</v>
+      </c>
+      <c r="L9" s="15">
+        <v>0.98442490847327502</v>
+      </c>
+      <c r="M9" s="12">
+        <v>11</v>
       </c>
       <c r="N9" s="14">
-        <v>43125</v>
+        <v>43133</v>
       </c>
       <c r="O9" s="12">
-        <v>2259.4</v>
+        <v>2368.0541871921182</v>
       </c>
       <c r="P9">
         <v>0.01</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>20</v>
+      <c r="A10" s="10">
+        <v>38</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>5</v>
@@ -1216,7 +1210,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E10" s="7">
         <v>2</v>
@@ -1227,37 +1221,37 @@
       <c r="G10" s="8">
         <v>12</v>
       </c>
-      <c r="H10" s="16">
-        <v>0.28741678076701066</v>
-      </c>
-      <c r="I10" s="16">
-        <v>0.44032739895047329</v>
-      </c>
-      <c r="J10" s="16">
-        <v>0.863552261978355</v>
-      </c>
-      <c r="K10" s="16">
-        <v>0.98157895585965094</v>
-      </c>
-      <c r="L10" s="16">
-        <v>0.9637034674677829</v>
-      </c>
-      <c r="M10" s="11">
-        <v>11</v>
+      <c r="H10" s="15">
+        <v>0.11389547250595437</v>
+      </c>
+      <c r="I10" s="15">
+        <v>0.40198233943894168</v>
+      </c>
+      <c r="J10" s="15">
+        <v>0.93788470371045773</v>
+      </c>
+      <c r="K10" s="15">
+        <v>0.94679421908849015</v>
+      </c>
+      <c r="L10" s="15">
+        <v>0.97266107566190241</v>
+      </c>
+      <c r="M10" s="12">
+        <v>0</v>
       </c>
       <c r="N10" s="14">
-        <v>43125</v>
+        <v>43129</v>
       </c>
       <c r="O10" s="12">
-        <v>2304.8250000000003</v>
+        <v>2055.1732673267325</v>
       </c>
       <c r="P10">
         <v>0.01</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>21</v>
+      <c r="A11" s="10">
+        <v>39</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>5</v>
@@ -1266,7 +1260,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E11" s="7">
         <v>3</v>
@@ -1277,87 +1271,87 @@
       <c r="G11" s="8">
         <v>12</v>
       </c>
-      <c r="H11" s="16">
-        <v>0.21660635228204098</v>
-      </c>
-      <c r="I11" s="16">
-        <v>0.29213775805217934</v>
-      </c>
-      <c r="J11" s="16">
-        <v>0.60406073067049937</v>
-      </c>
-      <c r="K11" s="16">
-        <v>0.91101435858154467</v>
-      </c>
-      <c r="L11" s="16">
-        <v>0.99457654583974886</v>
-      </c>
-      <c r="M11" s="11">
-        <v>12</v>
+      <c r="H11" s="15">
+        <v>0.10495677630284739</v>
+      </c>
+      <c r="I11" s="15">
+        <v>0.22354583401040304</v>
+      </c>
+      <c r="J11" s="15">
+        <v>0.52053921608252407</v>
+      </c>
+      <c r="K11" s="15">
+        <v>0.94723911252790927</v>
+      </c>
+      <c r="L11" s="15">
+        <v>1</v>
+      </c>
+      <c r="M11" s="12">
+        <v>1</v>
       </c>
       <c r="N11" s="14">
-        <v>43125</v>
+        <v>43129</v>
       </c>
       <c r="O11" s="12">
-        <v>2187.3869346733668</v>
+        <v>2083.4313725490197</v>
       </c>
       <c r="P11">
         <v>0.01</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>22</v>
+      <c r="A12" s="10">
+        <v>40</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C12" s="6">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="E12" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="G12" s="8">
-        <v>0</v>
-      </c>
-      <c r="H12" s="16">
-        <v>0.23431614457893668</v>
-      </c>
-      <c r="I12" s="16">
-        <v>0.23108882558698798</v>
-      </c>
-      <c r="J12" s="16">
-        <v>0.27517452636994272</v>
-      </c>
-      <c r="K12" s="16">
-        <v>0.30234761161988</v>
-      </c>
-      <c r="L12" s="16">
-        <v>0.35836876414979529</v>
-      </c>
-      <c r="M12" s="11">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="H12" s="15">
+        <v>0.29402194280463373</v>
+      </c>
+      <c r="I12" s="15">
+        <v>0.59279736430854302</v>
+      </c>
+      <c r="J12" s="15">
+        <v>0.95710225438465057</v>
+      </c>
+      <c r="K12" s="15">
+        <v>0.9502589059068054</v>
+      </c>
+      <c r="L12" s="15">
+        <v>0.97727067553649472</v>
+      </c>
+      <c r="M12" s="12">
+        <v>3</v>
       </c>
       <c r="N12" s="14">
-        <v>43125</v>
+        <v>43129</v>
       </c>
       <c r="O12" s="12">
-        <v>2336.4250000000002</v>
+        <v>2393.8190954773868</v>
       </c>
       <c r="P12">
         <v>0.01</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>23</v>
+      <c r="A13" s="10">
+        <v>40</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>5</v>
@@ -1366,7 +1360,7 @@
         <v>3</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E13" s="7">
         <v>1</v>
@@ -1377,29 +1371,29 @@
       <c r="G13" s="8">
         <v>12</v>
       </c>
-      <c r="H13" s="16">
-        <v>0.28286912427393568</v>
-      </c>
-      <c r="I13" s="16">
-        <v>0.5932863446941754</v>
-      </c>
-      <c r="J13" s="16">
-        <v>0.95667025928959537</v>
-      </c>
-      <c r="K13" s="16">
-        <v>0.95896394745104319</v>
-      </c>
-      <c r="L13" s="16">
-        <v>0.9620820982579561</v>
-      </c>
-      <c r="M13" s="11">
-        <v>14</v>
+      <c r="H13" s="15">
+        <v>0.14326916217312871</v>
+      </c>
+      <c r="I13" s="15">
+        <v>0.22116571770936133</v>
+      </c>
+      <c r="J13" s="15">
+        <v>0.39498960898769003</v>
+      </c>
+      <c r="K13" s="15">
+        <v>0.84560739540108898</v>
+      </c>
+      <c r="L13" s="15">
+        <v>0.91852167511390326</v>
+      </c>
+      <c r="M13" s="12">
+        <v>12</v>
       </c>
       <c r="N13" s="14">
-        <v>43125</v>
+        <v>43133</v>
       </c>
       <c r="O13" s="12">
-        <v>2048.0750000000003</v>
+        <v>2115.2249999999999</v>
       </c>
       <c r="P13">
         <v>0.01</v>
@@ -1407,7 +1401,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>5</v>
@@ -1416,7 +1410,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E14" s="7">
         <v>2</v>
@@ -1428,28 +1422,28 @@
         <v>12</v>
       </c>
       <c r="H14" s="15">
-        <v>0.11389547250595437</v>
+        <v>0.21510119483910037</v>
       </c>
       <c r="I14" s="15">
-        <v>0.40198233943894168</v>
+        <v>0.26784030641085771</v>
       </c>
       <c r="J14" s="15">
-        <v>0.93788470371045773</v>
+        <v>0.368960935542752</v>
       </c>
       <c r="K14" s="15">
-        <v>0.94679421908849015</v>
+        <v>0.70713027860865196</v>
       </c>
       <c r="L14" s="15">
-        <v>0.97266107566190241</v>
+        <v>0.97485061376055748</v>
       </c>
       <c r="M14" s="12">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="N14" s="14">
-        <v>43129</v>
+        <v>43133</v>
       </c>
       <c r="O14" s="12">
-        <v>2055.1732673267325</v>
+        <v>2276.708542713568</v>
       </c>
       <c r="P14">
         <v>0.01</v>
@@ -1457,7 +1451,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>5</v>
@@ -1466,7 +1460,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E15" s="7">
         <v>3</v>
@@ -1478,28 +1472,28 @@
         <v>12</v>
       </c>
       <c r="H15" s="15">
-        <v>0.10495677630284739</v>
+        <v>0.19173790208043537</v>
       </c>
       <c r="I15" s="15">
-        <v>0.22354583401040304</v>
+        <v>0.20309675684751127</v>
       </c>
       <c r="J15" s="15">
-        <v>0.52053921608252407</v>
+        <v>0.24687976699504002</v>
       </c>
       <c r="K15" s="15">
-        <v>0.94723911252790927</v>
+        <v>0.49999847959565641</v>
       </c>
       <c r="L15" s="15">
-        <v>1</v>
+        <v>0.96448205834093592</v>
       </c>
       <c r="M15" s="12">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="N15" s="14">
-        <v>43129</v>
+        <v>43133</v>
       </c>
       <c r="O15" s="12">
-        <v>2083.4313725490197</v>
+        <v>1992.7750000000001</v>
       </c>
       <c r="P15">
         <v>0.01</v>
@@ -1507,7 +1501,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>5</v>
@@ -1516,7 +1510,7 @@
         <v>3</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E16" s="7">
         <v>1</v>
@@ -1528,28 +1522,28 @@
         <v>12</v>
       </c>
       <c r="H16" s="15">
-        <v>0.29402194280463373</v>
+        <v>0.22697083283167832</v>
       </c>
       <c r="I16" s="15">
-        <v>0.59279736430854302</v>
+        <v>0.35877964305050836</v>
       </c>
       <c r="J16" s="15">
-        <v>0.95710225438465057</v>
+        <v>0.65275803786971642</v>
       </c>
       <c r="K16" s="15">
-        <v>0.9502589059068054</v>
+        <v>0.93769487072197466</v>
       </c>
       <c r="L16" s="15">
-        <v>0.97727067553649472</v>
+        <v>0.95490411646214624</v>
       </c>
       <c r="M16" s="12">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N16" s="14">
-        <v>43129</v>
+        <v>43133</v>
       </c>
       <c r="O16" s="12">
-        <v>2393.8190954773868</v>
+        <v>1828.5125628140704</v>
       </c>
       <c r="P16">
         <v>0.01</v>
@@ -1557,19 +1551,19 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>27</v>
       </c>
       <c r="E17" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>7</v>
@@ -1577,29 +1571,29 @@
       <c r="G17" s="8">
         <v>12</v>
       </c>
-      <c r="H17" s="15">
-        <v>0.11916911057185571</v>
-      </c>
-      <c r="I17" s="15">
-        <v>0.25784749413721103</v>
-      </c>
-      <c r="J17" s="15">
-        <v>0.53172546327210368</v>
-      </c>
-      <c r="K17" s="15">
-        <v>0.93770236315694111</v>
-      </c>
-      <c r="L17" s="15">
-        <v>1</v>
+      <c r="H17">
+        <v>0.27350382173483972</v>
+      </c>
+      <c r="I17">
+        <v>0.32767013802515432</v>
+      </c>
+      <c r="J17">
+        <v>0.69616424040213165</v>
+      </c>
+      <c r="K17">
+        <v>0.99749071275987988</v>
+      </c>
+      <c r="L17">
+        <v>1.0001854306939946</v>
       </c>
       <c r="M17" s="12">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="N17" s="14">
-        <v>43129</v>
+        <v>43133</v>
       </c>
       <c r="O17" s="12">
-        <v>2153.1372549019611</v>
+        <v>2109.9748743718592</v>
       </c>
       <c r="P17">
         <v>0.01</v>
@@ -1607,20 +1601,20 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="6">
+        <v>1</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="7">
         <v>3</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" s="7">
-        <v>1</v>
-      </c>
       <c r="F18" s="8" t="s">
         <v>7</v>
       </c>
@@ -1628,28 +1622,28 @@
         <v>12</v>
       </c>
       <c r="H18" s="15">
-        <v>0.18078260297798135</v>
+        <v>0.11916911057185571</v>
       </c>
       <c r="I18" s="15">
-        <v>0.50345207503170064</v>
+        <v>0.25784749413721103</v>
       </c>
       <c r="J18" s="15">
-        <v>0.93876585770149701</v>
+        <v>0.53172546327210368</v>
       </c>
       <c r="K18" s="15">
-        <v>0.96947048817903492</v>
+        <v>0.93770236315694111</v>
       </c>
       <c r="L18" s="15">
-        <v>0.97159753441671182</v>
+        <v>1</v>
       </c>
       <c r="M18" s="12">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N18" s="14">
         <v>43129</v>
       </c>
       <c r="O18" s="12">
-        <v>2038.5175879396986</v>
+        <v>2153.1372549019611</v>
       </c>
       <c r="P18">
         <v>0.01</v>
@@ -1657,19 +1651,19 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>29</v>
       </c>
       <c r="E19" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>7</v>
@@ -1678,28 +1672,28 @@
         <v>12</v>
       </c>
       <c r="H19" s="15">
-        <v>0.32951792175157096</v>
+        <v>0.18078260297798135</v>
       </c>
       <c r="I19" s="15">
-        <v>0.47884022253005371</v>
+        <v>0.50345207503170064</v>
       </c>
       <c r="J19" s="15">
-        <v>0.6465493334566037</v>
+        <v>0.93876585770149701</v>
       </c>
       <c r="K19" s="15">
-        <v>0.94070689522340445</v>
+        <v>0.96947048817903492</v>
       </c>
       <c r="L19" s="15">
-        <v>1</v>
+        <v>0.97159753441671182</v>
       </c>
       <c r="M19" s="12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N19" s="14">
         <v>43129</v>
       </c>
       <c r="O19" s="12">
-        <v>2233.7931034482758</v>
+        <v>2038.5175879396986</v>
       </c>
       <c r="P19">
         <v>0.01</v>
@@ -1707,19 +1701,19 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>29</v>
       </c>
       <c r="E20" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>7</v>
@@ -1728,28 +1722,28 @@
         <v>12</v>
       </c>
       <c r="H20" s="15">
-        <v>0.16778248808607574</v>
+        <v>0.32951792175157096</v>
       </c>
       <c r="I20" s="15">
-        <v>0.2314013120565197</v>
+        <v>0.47884022253005371</v>
       </c>
       <c r="J20" s="15">
-        <v>0.31826757627255536</v>
+        <v>0.6465493334566037</v>
       </c>
       <c r="K20" s="15">
-        <v>0.40762440376657733</v>
+        <v>0.94070689522340445</v>
       </c>
       <c r="L20" s="15">
-        <v>0.60728210166724328</v>
+        <v>1</v>
       </c>
       <c r="M20" s="12">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N20" s="14">
         <v>43129</v>
       </c>
       <c r="O20" s="12">
-        <v>1909.9646464646464</v>
+        <v>2233.7931034482758</v>
       </c>
       <c r="P20">
         <v>0.01</v>
@@ -1757,20 +1751,20 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="6">
+        <v>1</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="7">
         <v>3</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="7">
-        <v>1</v>
-      </c>
       <c r="F21" s="8" t="s">
         <v>7</v>
       </c>
@@ -1778,28 +1772,28 @@
         <v>12</v>
       </c>
       <c r="H21" s="15">
-        <v>0.3802573482961753</v>
+        <v>0.16778248808607574</v>
       </c>
       <c r="I21" s="15">
-        <v>0.87676848852953204</v>
+        <v>0.2314013120565197</v>
       </c>
       <c r="J21" s="15">
-        <v>0.95147975425234499</v>
+        <v>0.31826757627255536</v>
       </c>
       <c r="K21" s="15">
-        <v>0.93052621311663053</v>
+        <v>0.40762440376657733</v>
       </c>
       <c r="L21" s="15">
-        <v>0.96256312845190717</v>
+        <v>0.60728210166724328</v>
       </c>
       <c r="M21" s="12">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N21" s="14">
         <v>43129</v>
       </c>
       <c r="O21" s="12">
-        <v>2188.3000000000002</v>
+        <v>1909.9646464646464</v>
       </c>
       <c r="P21">
         <v>0.01</v>
@@ -1807,19 +1801,19 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>28</v>
       </c>
       <c r="E22" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>7</v>
@@ -1828,28 +1822,28 @@
         <v>12</v>
       </c>
       <c r="H22" s="15">
-        <v>0.28279430452016002</v>
+        <v>0.3802573482961753</v>
       </c>
       <c r="I22" s="15">
-        <v>0.77774200617259492</v>
+        <v>0.87676848852953204</v>
       </c>
       <c r="J22" s="15">
-        <v>0.98366665259062513</v>
+        <v>0.95147975425234499</v>
       </c>
       <c r="K22" s="15">
-        <v>0.99513540635883035</v>
+        <v>0.93052621311663053</v>
       </c>
       <c r="L22" s="15">
-        <v>1</v>
+        <v>0.96256312845190717</v>
       </c>
       <c r="M22" s="12">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N22" s="14">
         <v>43129</v>
       </c>
       <c r="O22" s="12">
-        <v>1934.7254901960787</v>
+        <v>2188.3000000000002</v>
       </c>
       <c r="P22">
         <v>0.01</v>
@@ -1857,19 +1851,19 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="E23" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>7</v>
@@ -1878,28 +1872,28 @@
         <v>12</v>
       </c>
       <c r="H23" s="15">
-        <v>8.8448772441250378E-2</v>
+        <v>0.28279430452016002</v>
       </c>
       <c r="I23" s="15">
-        <v>0.36900303806969204</v>
+        <v>0.77774200617259492</v>
       </c>
       <c r="J23" s="15">
-        <v>0.92378999312359533</v>
+        <v>0.98366665259062513</v>
       </c>
       <c r="K23" s="15">
-        <v>0.93264450938087895</v>
+        <v>0.99513540635883035</v>
       </c>
       <c r="L23" s="15">
-        <v>0.96509621425660008</v>
+        <v>1</v>
       </c>
       <c r="M23" s="12">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="N23" s="14">
-        <v>43133</v>
+        <v>43129</v>
       </c>
       <c r="O23" s="12">
-        <v>2057.9500000000003</v>
+        <v>1934.7254901960787</v>
       </c>
       <c r="P23">
         <v>0.01</v>
@@ -1907,19 +1901,19 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C24" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="E24" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>7</v>
@@ -1928,28 +1922,28 @@
         <v>12</v>
       </c>
       <c r="H24" s="15">
-        <v>0.19209965864266101</v>
+        <v>0.91444342420284064</v>
       </c>
       <c r="I24" s="15">
-        <v>0.48492784095629798</v>
+        <v>0.93210019400273991</v>
       </c>
       <c r="J24" s="15">
-        <v>0.9579800523816504</v>
+        <v>0.97009595721320585</v>
       </c>
       <c r="K24" s="15">
-        <v>1.0091528910794141</v>
+        <v>0.99508969945882009</v>
       </c>
       <c r="L24" s="15">
-        <v>1.0011138713772796</v>
+        <v>0.99792304079720162</v>
       </c>
       <c r="M24" s="12">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="N24" s="14">
-        <v>43133</v>
+        <v>43146</v>
       </c>
       <c r="O24" s="12">
-        <v>2162.7227722772277</v>
+        <v>2310.4520000000002</v>
       </c>
       <c r="P24">
         <v>0.01</v>
@@ -1957,19 +1951,19 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C25" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E25" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>7</v>
@@ -1978,28 +1972,28 @@
         <v>12</v>
       </c>
       <c r="H25" s="15">
-        <v>0.11327374860787404</v>
+        <v>0.50127869820561466</v>
       </c>
       <c r="I25" s="15">
-        <v>0.34762514691913898</v>
+        <v>0.93307332056181158</v>
       </c>
       <c r="J25" s="15">
-        <v>0.8354540499474985</v>
+        <v>0.34798807247824681</v>
       </c>
       <c r="K25" s="15">
-        <v>0.97479817949538916</v>
+        <v>0.98550638924848177</v>
       </c>
       <c r="L25" s="15">
-        <v>0.96599747056483165</v>
+        <v>0.99366352281872361</v>
       </c>
       <c r="M25" s="12">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="N25" s="14">
-        <v>43133</v>
+        <v>43146</v>
       </c>
       <c r="O25" s="12">
-        <v>2787.5</v>
+        <v>2248.3080808080808</v>
       </c>
       <c r="P25">
         <v>0.01</v>
@@ -2007,39 +2001,49 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C26" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E26" s="7">
+        <v>2</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" s="8">
+        <v>12</v>
+      </c>
+      <c r="H26" s="15">
+        <v>0.36768830661531876</v>
+      </c>
+      <c r="I26" s="15">
+        <v>0.86655257739735181</v>
+      </c>
+      <c r="J26" s="15">
+        <v>1</v>
+      </c>
+      <c r="K26" s="15">
+        <v>1</v>
+      </c>
+      <c r="L26" s="15">
+        <v>1</v>
+      </c>
+      <c r="M26" s="12">
         <v>0</v>
       </c>
-      <c r="F26" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G26" s="8">
-        <v>12</v>
-      </c>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="12">
-        <v>3</v>
-      </c>
       <c r="N26" s="14">
-        <v>43133</v>
+        <v>43151</v>
       </c>
       <c r="O26" s="12">
-        <v>2214.6844660194179</v>
+        <v>2234.9884526558894</v>
       </c>
       <c r="P26">
         <v>0.01</v>
@@ -2049,19 +2053,19 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E27" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>7</v>
@@ -2070,28 +2074,28 @@
         <v>12</v>
       </c>
       <c r="H27" s="15">
-        <v>0.32913075782129203</v>
+        <v>0.28768557440897274</v>
       </c>
       <c r="I27" s="15">
-        <v>0.40436473524431332</v>
+        <v>0.73381043204599383</v>
       </c>
       <c r="J27" s="15">
-        <v>0.62151391999376759</v>
+        <v>1</v>
       </c>
       <c r="K27" s="15">
-        <v>0.99099383606947011</v>
+        <v>0.99803585947280238</v>
       </c>
       <c r="L27" s="15">
-        <v>0.97395274989101532</v>
+        <v>0.99601237040060442</v>
       </c>
       <c r="M27" s="12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N27" s="14">
-        <v>43133</v>
+        <v>43151</v>
       </c>
       <c r="O27" s="12">
-        <v>1937.4849246231156</v>
+        <v>2320.4960835509137</v>
       </c>
       <c r="P27">
         <v>0.01</v>
@@ -2099,7 +2103,7 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>5</v>
@@ -2108,7 +2112,7 @@
         <v>3</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="E28" s="7">
         <v>1</v>
@@ -2120,28 +2124,28 @@
         <v>12</v>
       </c>
       <c r="H28" s="15">
-        <v>0.22697083283167832</v>
+        <v>0.48847059899398787</v>
       </c>
       <c r="I28" s="15">
-        <v>0.35877964305050836</v>
+        <v>0.93205302876170337</v>
       </c>
       <c r="J28" s="15">
-        <v>0.65275803786971642</v>
+        <v>0.99813369003560004</v>
       </c>
       <c r="K28" s="15">
-        <v>0.93769487072197466</v>
+        <v>0.995350440053552</v>
       </c>
       <c r="L28" s="15">
-        <v>0.95490411646214624</v>
+        <v>0.99953671547277778</v>
       </c>
       <c r="M28" s="12">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="N28" s="14">
-        <v>43133</v>
+        <v>43151</v>
       </c>
       <c r="O28" s="12">
-        <v>1828.5125628140704</v>
+        <v>2271.047227926078</v>
       </c>
       <c r="P28">
         <v>0.01</v>
@@ -2149,7 +2153,7 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>5</v>
@@ -2158,7 +2162,7 @@
         <v>2</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="E29" s="7">
         <v>2</v>
@@ -2170,28 +2174,28 @@
         <v>12</v>
       </c>
       <c r="H29" s="15">
-        <v>0.22020814845819869</v>
+        <v>0.41542222960626685</v>
       </c>
       <c r="I29" s="15">
-        <v>0.26914917351921069</v>
+        <v>0.71151262154585393</v>
       </c>
       <c r="J29" s="15">
-        <v>0.40724473288786356</v>
+        <v>0.99753350059226131</v>
       </c>
       <c r="K29" s="15">
-        <v>0.77601522752589736</v>
+        <v>1</v>
       </c>
       <c r="L29" s="15">
-        <v>1.0400614197627636</v>
+        <v>1</v>
       </c>
       <c r="M29" s="12">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="N29" s="14">
-        <v>43133</v>
+        <v>43151</v>
       </c>
       <c r="O29" s="12">
-        <v>2109.9748743718592</v>
+        <v>2552.3503737520696</v>
       </c>
       <c r="P29">
         <v>0.01</v>
@@ -2199,49 +2203,49 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C30" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E30" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="G30" s="8">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H30" s="15">
-        <v>0.24675021175493536</v>
+        <v>0.25439508455086418</v>
       </c>
       <c r="I30" s="15">
-        <v>0.28733107150260734</v>
+        <v>0.54680623436592934</v>
       </c>
       <c r="J30" s="15">
-        <v>0.49512127230716052</v>
+        <v>0.94983288251657516</v>
       </c>
       <c r="K30" s="15">
-        <v>0.8486639983684201</v>
+        <v>1</v>
       </c>
       <c r="L30" s="15">
-        <v>0.93491784964297076</v>
+        <v>1</v>
       </c>
       <c r="M30" s="12">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="N30" s="14">
-        <v>43133</v>
+        <v>43151</v>
       </c>
       <c r="O30" s="12">
-        <v>1975</v>
+        <v>1868.8214643931797</v>
       </c>
       <c r="P30">
         <v>0.01</v>
@@ -2249,19 +2253,19 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C31" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="E31" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>7</v>
@@ -2270,28 +2274,28 @@
         <v>12</v>
       </c>
       <c r="H31" s="15">
-        <v>0.20494025535697469</v>
+        <v>0.42896103463403357</v>
       </c>
       <c r="I31" s="15">
-        <v>0.32319328315160306</v>
+        <v>0.82130655029849109</v>
       </c>
       <c r="J31" s="15">
-        <v>0.74540804107981595</v>
+        <v>0.95553190654897913</v>
       </c>
       <c r="K31" s="15">
-        <v>0.95552327266352266</v>
+        <v>0.94900734808188414</v>
       </c>
       <c r="L31" s="15">
-        <v>0.97407546577591397</v>
+        <v>0.96642058433149725</v>
       </c>
       <c r="M31" s="12">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="N31" s="14">
-        <v>43133</v>
+        <v>43151</v>
       </c>
       <c r="O31" s="12">
-        <v>2008.575</v>
+        <v>2548.2590564236548</v>
       </c>
       <c r="P31">
         <v>0.01</v>
@@ -2299,7 +2303,7 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
-        <v>33</v>
+        <v>106</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>5</v>
@@ -2308,7 +2312,7 @@
         <v>3</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="E32" s="7">
         <v>1</v>
@@ -2320,28 +2324,28 @@
         <v>12</v>
       </c>
       <c r="H32" s="15">
-        <v>0.38772385066941001</v>
+        <v>0.5014964584336209</v>
       </c>
       <c r="I32" s="15">
-        <v>0.5049664106522217</v>
+        <v>0.49683253182655912</v>
       </c>
       <c r="J32" s="15">
-        <v>0.81580047533790245</v>
+        <v>0.71478915039649715</v>
       </c>
       <c r="K32" s="15">
-        <v>0.98184797965604254</v>
+        <v>0.98262958566389547</v>
       </c>
       <c r="L32" s="15">
-        <v>0.98442490847327502</v>
+        <v>0.98581718301205246</v>
       </c>
       <c r="M32" s="12">
         <v>11</v>
       </c>
       <c r="N32" s="14">
-        <v>43133</v>
+        <v>43146</v>
       </c>
       <c r="O32" s="12">
-        <v>2368.0541871921182</v>
+        <v>2401.1330049261087</v>
       </c>
       <c r="P32">
         <v>0.01</v>
@@ -2349,19 +2353,19 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
-        <v>40</v>
+        <v>107</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C33" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="E33" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>7</v>
@@ -2370,28 +2374,28 @@
         <v>12</v>
       </c>
       <c r="H33" s="15">
-        <v>0.14326916217312871</v>
+        <v>0.28450735289031309</v>
       </c>
       <c r="I33" s="15">
-        <v>0.22116571770936133</v>
+        <v>0.26295971209097374</v>
       </c>
       <c r="J33" s="15">
-        <v>0.39498960898769003</v>
+        <v>0.28997469374379092</v>
       </c>
       <c r="K33" s="15">
-        <v>0.84560739540108898</v>
+        <v>0.98103578698981697</v>
       </c>
       <c r="L33" s="15">
-        <v>0.91852167511390326</v>
+        <v>0.40081097757936773</v>
       </c>
       <c r="M33" s="12">
         <v>12</v>
       </c>
       <c r="N33" s="14">
-        <v>43133</v>
+        <v>43146</v>
       </c>
       <c r="O33" s="12">
-        <v>2115.2249999999999</v>
+        <v>2192.9310344827586</v>
       </c>
       <c r="P33">
         <v>0.01</v>
@@ -2399,19 +2403,19 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
-        <v>41</v>
+        <v>108</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C34" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="E34" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>7</v>
@@ -2420,28 +2424,28 @@
         <v>12</v>
       </c>
       <c r="H34" s="15">
-        <v>0.21510119483910037</v>
+        <v>0.31290627743941185</v>
       </c>
       <c r="I34" s="15">
-        <v>0.26784030641085771</v>
+        <v>0.32312071613838772</v>
       </c>
       <c r="J34" s="15">
-        <v>0.368960935542752</v>
+        <v>0.33586916126941907</v>
       </c>
       <c r="K34" s="15">
-        <v>0.70713027860865196</v>
+        <v>0.34005652218335847</v>
       </c>
       <c r="L34" s="15">
-        <v>0.97485061376055748</v>
+        <v>0.4179278276779293</v>
       </c>
       <c r="M34" s="12">
         <v>13</v>
       </c>
       <c r="N34" s="14">
-        <v>43133</v>
+        <v>43146</v>
       </c>
       <c r="O34" s="12">
-        <v>2276.708542713568</v>
+        <v>2268.8177339901476</v>
       </c>
       <c r="P34">
         <v>0.01</v>
@@ -2449,49 +2453,49 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
-        <v>42</v>
+        <v>112</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C35" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E35" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="G35" s="8">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="H35" s="15">
-        <v>0.19173790208043537</v>
+        <v>0.25474137100038258</v>
       </c>
       <c r="I35" s="15">
-        <v>0.20309675684751127</v>
+        <v>0.27369478498386762</v>
       </c>
       <c r="J35" s="15">
-        <v>0.24687976699504002</v>
+        <v>0.44019551905976823</v>
       </c>
       <c r="K35" s="15">
-        <v>0.49999847959565641</v>
+        <v>0.7548640002292637</v>
       </c>
       <c r="L35" s="15">
-        <v>0.96448205834093592</v>
+        <v>0.96762143203036266</v>
       </c>
       <c r="M35" s="12">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="N35" s="14">
-        <v>43133</v>
+        <v>43146</v>
       </c>
       <c r="O35" s="12">
-        <v>1992.7750000000001</v>
+        <v>2182.375</v>
       </c>
       <c r="P35">
         <v>0.01</v>
@@ -2499,7 +2503,7 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>5</v>
@@ -2508,7 +2512,7 @@
         <v>2</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E36" s="7">
         <v>2</v>
@@ -2520,28 +2524,28 @@
         <v>0</v>
       </c>
       <c r="H36" s="15">
-        <v>0.25474137100038258</v>
+        <v>0</v>
       </c>
       <c r="I36" s="15">
-        <v>0.27369478498386762</v>
+        <v>0</v>
       </c>
       <c r="J36" s="15">
-        <v>0.44019551905976823</v>
+        <v>8.4220949637530282E-2</v>
       </c>
       <c r="K36" s="15">
-        <v>0.7548640002292637</v>
+        <v>0.33582296571479864</v>
       </c>
       <c r="L36" s="15">
-        <v>0.96762143203036266</v>
+        <v>0.7704341544961314</v>
       </c>
       <c r="M36" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N36" s="14">
         <v>43146</v>
       </c>
       <c r="O36" s="12">
-        <v>2182.375</v>
+        <v>2156.7000000000003</v>
       </c>
       <c r="P36">
         <v>0.01</v>
@@ -2549,7 +2553,7 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>5</v>
@@ -2558,7 +2562,7 @@
         <v>2</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E37" s="7">
         <v>2</v>
@@ -2570,28 +2574,28 @@
         <v>0</v>
       </c>
       <c r="H37" s="15">
-        <v>0</v>
+        <v>0.32486472532903349</v>
       </c>
       <c r="I37" s="15">
-        <v>0</v>
+        <v>0.37028222247756082</v>
       </c>
       <c r="J37" s="15">
-        <v>8.4220949637530282E-2</v>
+        <v>0.47627843442985957</v>
       </c>
       <c r="K37" s="15">
-        <v>0.33582296571479864</v>
+        <v>0.73334412337764687</v>
       </c>
       <c r="L37" s="15">
-        <v>0.7704341544961314</v>
+        <v>1</v>
       </c>
       <c r="M37" s="12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N37" s="14">
         <v>43146</v>
       </c>
       <c r="O37" s="12">
-        <v>2156.7000000000003</v>
+        <v>2305.7881773399017</v>
       </c>
       <c r="P37">
         <v>0.01</v>
@@ -2599,7 +2603,7 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>5</v>
@@ -2608,7 +2612,7 @@
         <v>2</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="E38" s="7">
         <v>2</v>
@@ -2620,28 +2624,28 @@
         <v>0</v>
       </c>
       <c r="H38" s="15">
-        <v>0.32486472532903349</v>
+        <v>0.4184695515499291</v>
       </c>
       <c r="I38" s="15">
-        <v>0.37028222247756082</v>
+        <v>0.40557224913681822</v>
       </c>
       <c r="J38" s="15">
-        <v>0.47627843442985957</v>
+        <v>0.6865329581113212</v>
       </c>
       <c r="K38" s="15">
-        <v>0.73334412337764687</v>
+        <v>0.99858429846274077</v>
       </c>
       <c r="L38" s="15">
-        <v>1</v>
+        <v>1.0256439131903667</v>
       </c>
       <c r="M38" s="12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N38" s="14">
         <v>43146</v>
       </c>
       <c r="O38" s="12">
-        <v>2305.7881773399017</v>
+        <v>1973.0637254901965</v>
       </c>
       <c r="P38">
         <v>0.01</v>
@@ -2649,7 +2653,7 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="10">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>5</v>
@@ -2658,7 +2662,7 @@
         <v>2</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="E39" s="7">
         <v>2</v>
@@ -2670,28 +2674,28 @@
         <v>0</v>
       </c>
       <c r="H39" s="15">
-        <v>0.4184695515499291</v>
+        <v>0.28640914268171236</v>
       </c>
       <c r="I39" s="15">
-        <v>0.40557224913681822</v>
+        <v>0.28671645096120585</v>
       </c>
       <c r="J39" s="15">
-        <v>0.6865329581113212</v>
+        <v>0.63860296303490116</v>
       </c>
       <c r="K39" s="15">
-        <v>0.99858429846274077</v>
+        <v>0.93441702317447117</v>
       </c>
       <c r="L39" s="15">
-        <v>1.0256439131903667</v>
+        <v>0.98793362948894503</v>
       </c>
       <c r="M39" s="12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N39" s="14">
         <v>43146</v>
       </c>
       <c r="O39" s="12">
-        <v>1973.0637254901965</v>
+        <v>1832.8</v>
       </c>
       <c r="P39">
         <v>0.01</v>
@@ -2699,7 +2703,7 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="10">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>5</v>
@@ -2708,7 +2712,7 @@
         <v>2</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E40" s="7">
         <v>2</v>
@@ -2720,28 +2724,28 @@
         <v>0</v>
       </c>
       <c r="H40" s="15">
-        <v>0.28640914268171236</v>
+        <v>0.1982856950846246</v>
       </c>
       <c r="I40" s="15">
-        <v>0.28671645096120585</v>
+        <v>0.243954390162158</v>
       </c>
       <c r="J40" s="15">
-        <v>0.63860296303490116</v>
+        <v>0.34226455279070156</v>
       </c>
       <c r="K40" s="15">
-        <v>0.93441702317447117</v>
+        <v>0.45662317465069813</v>
       </c>
       <c r="L40" s="15">
-        <v>0.98793362948894503</v>
+        <v>0.68893048189446604</v>
       </c>
       <c r="M40" s="12">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N40" s="14">
         <v>43146</v>
       </c>
       <c r="O40" s="12">
-        <v>1832.8</v>
+        <v>2178.4250000000002</v>
       </c>
       <c r="P40">
         <v>0.01</v>
@@ -2749,7 +2753,7 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="10">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>5</v>
@@ -2758,7 +2762,7 @@
         <v>2</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E41" s="7">
         <v>2</v>
@@ -2770,28 +2774,28 @@
         <v>0</v>
       </c>
       <c r="H41" s="15">
-        <v>0.1982856950846246</v>
+        <v>0.11676707434621185</v>
       </c>
       <c r="I41" s="15">
-        <v>0.243954390162158</v>
+        <v>0.21633707409019648</v>
       </c>
       <c r="J41" s="15">
-        <v>0.34226455279070156</v>
+        <v>0.49234325744542856</v>
       </c>
       <c r="K41" s="15">
-        <v>0.45662317465069813</v>
+        <v>0.49234325744542856</v>
       </c>
       <c r="L41" s="15">
-        <v>0.68893048189446604</v>
+        <v>0.94799569405847739</v>
       </c>
       <c r="M41" s="12">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N41" s="14">
         <v>43146</v>
       </c>
       <c r="O41" s="12">
-        <v>2178.4250000000002</v>
+        <v>2047.3514851485149</v>
       </c>
       <c r="P41">
         <v>0.01</v>
@@ -2799,7 +2803,7 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="10">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>5</v>
@@ -2808,7 +2812,7 @@
         <v>2</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E42" s="7">
         <v>2</v>
@@ -2820,28 +2824,28 @@
         <v>0</v>
       </c>
       <c r="H42" s="15">
-        <v>0.11676707434621185</v>
+        <v>0.32476352087129468</v>
       </c>
       <c r="I42" s="15">
-        <v>0.21633707409019648</v>
+        <v>0.33428255417535369</v>
       </c>
       <c r="J42" s="15">
-        <v>0.49234325744542856</v>
+        <v>0.52434018857684717</v>
       </c>
       <c r="K42" s="15">
-        <v>0.49234325744542856</v>
+        <v>0.86076448888796664</v>
       </c>
       <c r="L42" s="15">
-        <v>0.94799569405847739</v>
+        <v>1.0098554115550948</v>
       </c>
       <c r="M42" s="12">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="N42" s="14">
         <v>43146</v>
       </c>
       <c r="O42" s="12">
-        <v>2047.3514851485149</v>
+        <v>2283.9603960396039</v>
       </c>
       <c r="P42">
         <v>0.01</v>
@@ -2849,7 +2853,7 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="10">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>5</v>
@@ -2858,7 +2862,7 @@
         <v>2</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="E43" s="7">
         <v>2</v>
@@ -2870,28 +2874,28 @@
         <v>0</v>
       </c>
       <c r="H43" s="15">
-        <v>0.32476352087129468</v>
+        <v>0.26307272374474999</v>
       </c>
       <c r="I43" s="15">
-        <v>0.33428255417535369</v>
+        <v>0.32371296258478305</v>
       </c>
       <c r="J43" s="15">
-        <v>0.52434018857684717</v>
+        <v>0.56235063802579088</v>
       </c>
       <c r="K43" s="15">
-        <v>0.86076448888796664</v>
+        <v>0.96278455730407009</v>
       </c>
       <c r="L43" s="15">
-        <v>1.0098554115550948</v>
+        <v>1</v>
       </c>
       <c r="M43" s="12">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="N43" s="14">
-        <v>43146</v>
+        <v>43151</v>
       </c>
       <c r="O43" s="12">
-        <v>2283.9603960396039</v>
+        <v>2165.170511534604</v>
       </c>
       <c r="P43">
         <v>0.01</v>
@@ -2899,49 +2903,49 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="10">
-        <v>57</v>
+        <v>121</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C44" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="E44" s="7">
+        <v>2</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G44" s="8">
+        <v>0</v>
+      </c>
+      <c r="H44" s="15">
+        <v>0.30255220585871595</v>
+      </c>
+      <c r="I44" s="15">
+        <v>0.35177982287483683</v>
+      </c>
+      <c r="J44" s="15">
+        <v>0.59645509438324507</v>
+      </c>
+      <c r="K44" s="15">
+        <v>0.96832620907498024</v>
+      </c>
+      <c r="L44" s="15">
+        <v>0.96853461960354703</v>
+      </c>
+      <c r="M44" s="12">
         <v>3</v>
       </c>
-      <c r="F44" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G44" s="8">
-        <v>12</v>
-      </c>
-      <c r="H44" s="15">
-        <v>0.91444342420284064</v>
-      </c>
-      <c r="I44" s="15">
-        <v>0.93210019400273991</v>
-      </c>
-      <c r="J44" s="15">
-        <v>0.97009595721320585</v>
-      </c>
-      <c r="K44" s="15">
-        <v>0.99508969945882009</v>
-      </c>
-      <c r="L44" s="15">
-        <v>0.99792304079720162</v>
-      </c>
-      <c r="M44" s="12">
-        <v>10</v>
-      </c>
       <c r="N44" s="14">
-        <v>43146</v>
+        <v>43151</v>
       </c>
       <c r="O44" s="12">
-        <v>2310.4520000000002</v>
+        <v>2465.6505800231002</v>
       </c>
       <c r="P44">
         <v>0.01</v>
@@ -2949,49 +2953,49 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="10">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C45" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E45" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="G45" s="8">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="H45" s="15">
-        <v>0.5014964584336209</v>
+        <v>0.30267584920745483</v>
       </c>
       <c r="I45" s="15">
-        <v>0.49683253182655912</v>
+        <v>0.39615455146703776</v>
       </c>
       <c r="J45" s="15">
-        <v>0.71478915039649715</v>
+        <v>0.66752801391145289</v>
       </c>
       <c r="K45" s="15">
-        <v>0.98262958566389547</v>
+        <v>0.99885283713292361</v>
       </c>
       <c r="L45" s="15">
-        <v>0.98581718301205246</v>
+        <v>0.99535831883300618</v>
       </c>
       <c r="M45" s="12">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="N45" s="14">
-        <v>43146</v>
+        <v>43151</v>
       </c>
       <c r="O45" s="12">
-        <v>2401.1330049261087</v>
+        <v>1961.7690021659196</v>
       </c>
       <c r="P45">
         <v>0.01</v>
@@ -2999,7 +3003,7 @@
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="10">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>5</v>
@@ -3008,40 +3012,40 @@
         <v>2</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="E46" s="7">
         <v>2</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="G46" s="8">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="H46" s="15">
-        <v>0.28450735289031309</v>
+        <v>0.22358339951050801</v>
       </c>
       <c r="I46" s="15">
-        <v>0.26295971209097374</v>
+        <v>0.31949703331092766</v>
       </c>
       <c r="J46" s="15">
-        <v>0.28997469374379092</v>
+        <v>0.63491193064385332</v>
       </c>
       <c r="K46" s="15">
-        <v>0.98103578698981697</v>
+        <v>0.9375577101334901</v>
       </c>
       <c r="L46" s="15">
-        <v>0.40081097757936773</v>
+        <v>0.97410363869288885</v>
       </c>
       <c r="M46" s="12">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="N46" s="14">
-        <v>43146</v>
+        <v>43151</v>
       </c>
       <c r="O46" s="12">
-        <v>2192.9310344827586</v>
+        <v>1829.3480996727917</v>
       </c>
       <c r="P46">
         <v>0.01</v>
@@ -3049,19 +3053,19 @@
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="10">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C47" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E47" s="7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F47" s="8" t="s">
         <v>7</v>
@@ -3070,28 +3074,28 @@
         <v>12</v>
       </c>
       <c r="H47" s="15">
-        <v>0.31290627743941185</v>
+        <v>0.22717879178441977</v>
       </c>
       <c r="I47" s="15">
-        <v>0.32312071613838772</v>
+        <v>0.20244056777673425</v>
       </c>
       <c r="J47" s="15">
-        <v>0.33586916126941907</v>
+        <v>0.25746916611770676</v>
       </c>
       <c r="K47" s="15">
-        <v>0.34005652218335847</v>
+        <v>0.28910792035817395</v>
       </c>
       <c r="L47" s="15">
-        <v>0.4179278276779293</v>
+        <v>0.43806356081658154</v>
       </c>
       <c r="M47" s="12">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="N47" s="14">
-        <v>43146</v>
+        <v>43151</v>
       </c>
       <c r="O47" s="12">
-        <v>2268.8177339901476</v>
+        <v>2333.99209486166</v>
       </c>
       <c r="P47">
         <v>0.01</v>
@@ -3099,49 +3103,49 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="10">
-        <v>58</v>
+        <v>125</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C48" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="E48" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="G48" s="8">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="H48" s="15">
-        <v>0.50127869820561466</v>
+        <v>9.335457974021566E-2</v>
       </c>
       <c r="I48" s="15">
-        <v>0.93307332056181158</v>
+        <v>0.10825248072024335</v>
       </c>
       <c r="J48" s="15">
-        <v>0.34798807247824681</v>
+        <v>9.1898124600874806E-2</v>
       </c>
       <c r="K48" s="15">
-        <v>0.98550638924848177</v>
+        <v>9.8328274279023242E-2</v>
       </c>
       <c r="L48" s="15">
-        <v>0.99366352281872361</v>
+        <v>0.12613640401722154</v>
       </c>
       <c r="M48" s="12">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="N48" s="14">
-        <v>43146</v>
+        <v>43151</v>
       </c>
       <c r="O48" s="12">
-        <v>2248.3080808080808</v>
+        <v>1990.7793578212149</v>
       </c>
       <c r="P48">
         <v>0.01</v>
@@ -3149,34 +3153,34 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="10">
-        <v>59</v>
+        <v>126</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C49" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="E49" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="G49" s="8">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="H49" s="15">
-        <v>0.36768830661531876</v>
+        <v>0.18068926339384092</v>
       </c>
       <c r="I49" s="15">
-        <v>0.86655257739735181</v>
+        <v>0.27632489613701899</v>
       </c>
       <c r="J49" s="15">
-        <v>1</v>
+        <v>0.70273394092228292</v>
       </c>
       <c r="K49" s="15">
         <v>1</v>
@@ -3185,183 +3189,183 @@
         <v>1</v>
       </c>
       <c r="M49" s="12">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="N49" s="14">
         <v>43151</v>
       </c>
       <c r="O49" s="12">
-        <v>2234.9884526558894</v>
+        <v>2232.9357522301293</v>
       </c>
       <c r="P49">
         <v>0.01</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A50" s="10">
-        <v>60</v>
+      <c r="A50" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C50" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="E50" s="7">
+        <v>1</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G50" s="8">
+        <v>12</v>
+      </c>
+      <c r="H50" s="16">
+        <v>9.4557951106624946E-2</v>
+      </c>
+      <c r="I50" s="16">
+        <v>0.1516853288512657</v>
+      </c>
+      <c r="J50" s="16">
+        <v>0.42895787388935297</v>
+      </c>
+      <c r="K50" s="16">
+        <v>0.95785891995849859</v>
+      </c>
+      <c r="L50" s="16">
+        <v>0.98499562083574521</v>
+      </c>
+      <c r="M50" s="11">
+        <v>0</v>
+      </c>
+      <c r="N50" s="14">
+        <v>43125</v>
+      </c>
+      <c r="O50" s="12">
+        <v>2092.9104477611941</v>
+      </c>
+      <c r="P50">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A51" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="6">
+        <v>2</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51" s="7">
+        <v>2</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G51" s="8">
+        <v>12</v>
+      </c>
+      <c r="H51" s="16">
+        <v>0.1195358705393363</v>
+      </c>
+      <c r="I51" s="16">
+        <v>0.13020674324129303</v>
+      </c>
+      <c r="J51" s="16">
+        <v>0.26005971336636069</v>
+      </c>
+      <c r="K51" s="16">
+        <v>0.61923951149020506</v>
+      </c>
+      <c r="L51" s="16">
+        <v>0.9877742331075684</v>
+      </c>
+      <c r="M51" s="11">
+        <v>1</v>
+      </c>
+      <c r="N51" s="14">
+        <v>43125</v>
+      </c>
+      <c r="O51" s="12">
+        <v>2176.4500000000003</v>
+      </c>
+      <c r="P51">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A52" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" s="6">
+        <v>1</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" s="7">
         <v>3</v>
       </c>
-      <c r="F50" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G50" s="8">
-        <v>12</v>
-      </c>
-      <c r="H50" s="15">
-        <v>0.28768557440897274</v>
-      </c>
-      <c r="I50" s="15">
-        <v>0.73381043204599383</v>
-      </c>
-      <c r="J50" s="15">
-        <v>1</v>
-      </c>
-      <c r="K50" s="15">
-        <v>0.99803585947280238</v>
-      </c>
-      <c r="L50" s="15">
-        <v>0.99601237040060442</v>
-      </c>
-      <c r="M50" s="12">
-        <v>1</v>
-      </c>
-      <c r="N50" s="14">
-        <v>43151</v>
-      </c>
-      <c r="O50" s="12">
-        <v>2320.4960835509137</v>
-      </c>
-      <c r="P50">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A51" s="10">
-        <v>120</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C51" s="6">
-        <v>2</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E51" s="7">
-        <v>2</v>
-      </c>
-      <c r="F51" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G51" s="8">
+      <c r="F52" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G52" s="8">
+        <v>12</v>
+      </c>
+      <c r="H52" s="16">
+        <v>0.19121111974535329</v>
+      </c>
+      <c r="I52" s="16">
+        <v>0.20612223570706134</v>
+      </c>
+      <c r="J52" s="16">
+        <v>0.27641542918024836</v>
+      </c>
+      <c r="K52" s="16">
+        <v>0.49135286954756102</v>
+      </c>
+      <c r="L52" s="16">
+        <v>0.86123370634274699</v>
+      </c>
+      <c r="M52" s="11">
+        <v>3</v>
+      </c>
+      <c r="N52" s="14">
+        <v>43125</v>
+      </c>
+      <c r="O52" s="12">
+        <v>2354.2000000000003</v>
+      </c>
+      <c r="P52">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A53" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="6">
+        <v>4</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E53" s="7">
         <v>0</v>
-      </c>
-      <c r="H51" s="15">
-        <v>0.26307272374474999</v>
-      </c>
-      <c r="I51" s="15">
-        <v>0.32371296258478305</v>
-      </c>
-      <c r="J51" s="15">
-        <v>0.56235063802579088</v>
-      </c>
-      <c r="K51" s="15">
-        <v>0.96278455730407009</v>
-      </c>
-      <c r="L51" s="15">
-        <v>1</v>
-      </c>
-      <c r="M51" s="12">
-        <v>2</v>
-      </c>
-      <c r="N51" s="14">
-        <v>43151</v>
-      </c>
-      <c r="O51" s="12">
-        <v>2165.170511534604</v>
-      </c>
-      <c r="P51">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A52" s="10">
-        <v>121</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C52" s="6">
-        <v>2</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E52" s="7">
-        <v>2</v>
-      </c>
-      <c r="F52" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G52" s="8">
-        <v>0</v>
-      </c>
-      <c r="H52" s="15">
-        <v>0.30255220585871595</v>
-      </c>
-      <c r="I52" s="15">
-        <v>0.35177982287483683</v>
-      </c>
-      <c r="J52" s="15">
-        <v>0.59645509438324507</v>
-      </c>
-      <c r="K52" s="15">
-        <v>0.96832620907498024</v>
-      </c>
-      <c r="L52" s="15">
-        <v>0.96853461960354703</v>
-      </c>
-      <c r="M52" s="12">
-        <v>3</v>
-      </c>
-      <c r="N52" s="14">
-        <v>43151</v>
-      </c>
-      <c r="O52" s="12">
-        <v>2465.6505800231002</v>
-      </c>
-      <c r="P52">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A53" s="10">
-        <v>122</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" s="6">
-        <v>2</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E53" s="7">
-        <v>2</v>
       </c>
       <c r="F53" s="8" t="s">
         <v>46</v>
@@ -3369,387 +3373,387 @@
       <c r="G53" s="8">
         <v>0</v>
       </c>
-      <c r="H53" s="15">
-        <v>0.30267584920745483</v>
-      </c>
-      <c r="I53" s="15">
-        <v>0.39615455146703776</v>
-      </c>
-      <c r="J53" s="15">
-        <v>0.66752801391145289</v>
-      </c>
-      <c r="K53" s="15">
-        <v>0.99885283713292361</v>
-      </c>
-      <c r="L53" s="15">
-        <v>0.99535831883300618</v>
-      </c>
-      <c r="M53" s="12">
+      <c r="H53" s="16">
+        <v>0.26671957824088333</v>
+      </c>
+      <c r="I53" s="16">
+        <v>0.4611335403017584</v>
+      </c>
+      <c r="J53" s="16">
+        <v>0.94082183810715747</v>
+      </c>
+      <c r="K53" s="16">
+        <v>1</v>
+      </c>
+      <c r="L53" s="16">
+        <v>1</v>
+      </c>
+      <c r="M53" s="11">
         <v>4</v>
       </c>
       <c r="N53" s="14">
-        <v>43151</v>
+        <v>43125</v>
       </c>
       <c r="O53" s="12">
-        <v>1961.7690021659196</v>
+        <v>1925.625</v>
       </c>
       <c r="P53">
         <v>0.01</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A54" s="10">
-        <v>123</v>
+      <c r="A54" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C54" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E54" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F54" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G54" s="8">
+        <v>12</v>
+      </c>
+      <c r="H54" s="16">
+        <v>0.50969447771133602</v>
+      </c>
+      <c r="I54" s="16">
+        <v>0.94519530746047431</v>
+      </c>
+      <c r="J54" s="16">
+        <v>0.96635511610319114</v>
+      </c>
+      <c r="K54" s="16">
+        <v>0.95752529870093561</v>
+      </c>
+      <c r="L54" s="16">
+        <v>0.9576437682443496</v>
+      </c>
+      <c r="M54" s="11">
+        <v>5</v>
+      </c>
+      <c r="N54" s="14">
+        <v>43125</v>
+      </c>
+      <c r="O54" s="12">
+        <v>1825.8875</v>
+      </c>
+      <c r="P54">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A55" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" s="6">
+        <v>2</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" s="7">
+        <v>2</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G55" s="8">
+        <v>12</v>
+      </c>
+      <c r="H55" s="16">
+        <v>0.46819270517182704</v>
+      </c>
+      <c r="I55" s="16">
+        <v>0.89407361672624663</v>
+      </c>
+      <c r="J55" s="16">
+        <v>1</v>
+      </c>
+      <c r="K55" s="16">
+        <v>1</v>
+      </c>
+      <c r="L55" s="16">
+        <v>1</v>
+      </c>
+      <c r="M55" s="11">
+        <v>6</v>
+      </c>
+      <c r="N55" s="14">
+        <v>43125</v>
+      </c>
+      <c r="O55" s="12">
+        <v>2366.0301507537688</v>
+      </c>
+      <c r="P55">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" s="6">
+        <v>1</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" s="7">
+        <v>3</v>
+      </c>
+      <c r="F56" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G56" s="8">
+        <v>12</v>
+      </c>
+      <c r="H56" s="16">
+        <v>0.39237353123262569</v>
+      </c>
+      <c r="I56" s="16">
+        <v>0.84077737958456444</v>
+      </c>
+      <c r="J56" s="16">
+        <v>1</v>
+      </c>
+      <c r="K56" s="16">
+        <v>1</v>
+      </c>
+      <c r="L56" s="16">
+        <v>1</v>
+      </c>
+      <c r="M56" s="11">
+        <v>7</v>
+      </c>
+      <c r="N56" s="14">
+        <v>43125</v>
+      </c>
+      <c r="O56" s="12">
+        <v>1986.85</v>
+      </c>
+      <c r="P56">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A57" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" s="6">
+        <v>3</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="7">
+        <v>1</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G57" s="8">
+        <v>12</v>
+      </c>
+      <c r="H57" s="16">
+        <v>0.53459733253159325</v>
+      </c>
+      <c r="I57" s="16">
+        <v>0.97504215970422059</v>
+      </c>
+      <c r="J57" s="16">
+        <v>1</v>
+      </c>
+      <c r="K57" s="16">
+        <v>1</v>
+      </c>
+      <c r="L57" s="16">
+        <v>1</v>
+      </c>
+      <c r="M57" s="11">
+        <v>9</v>
+      </c>
+      <c r="N57" s="14">
+        <v>43125</v>
+      </c>
+      <c r="O57" s="12">
+        <v>2259.4</v>
+      </c>
+      <c r="P57">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A58" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" s="6">
+        <v>2</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" s="7">
+        <v>2</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G58" s="8">
+        <v>12</v>
+      </c>
+      <c r="H58" s="16">
+        <v>0.28741678076701066</v>
+      </c>
+      <c r="I58" s="16">
+        <v>0.44032739895047329</v>
+      </c>
+      <c r="J58" s="16">
+        <v>0.863552261978355</v>
+      </c>
+      <c r="K58" s="16">
+        <v>0.98157895585965094</v>
+      </c>
+      <c r="L58" s="16">
+        <v>0.9637034674677829</v>
+      </c>
+      <c r="M58" s="11">
+        <v>11</v>
+      </c>
+      <c r="N58" s="14">
+        <v>43125</v>
+      </c>
+      <c r="O58" s="12">
+        <v>2304.8250000000003</v>
+      </c>
+      <c r="P58">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A59" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" s="6">
+        <v>1</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" s="7">
+        <v>3</v>
+      </c>
+      <c r="F59" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G59" s="8">
+        <v>12</v>
+      </c>
+      <c r="H59" s="16">
+        <v>0.21660635228204098</v>
+      </c>
+      <c r="I59" s="16">
+        <v>0.29213775805217934</v>
+      </c>
+      <c r="J59" s="16">
+        <v>0.60406073067049937</v>
+      </c>
+      <c r="K59" s="16">
+        <v>0.91101435858154467</v>
+      </c>
+      <c r="L59" s="16">
+        <v>0.99457654583974886</v>
+      </c>
+      <c r="M59" s="11">
+        <v>12</v>
+      </c>
+      <c r="N59" s="14">
+        <v>43125</v>
+      </c>
+      <c r="O59" s="12">
+        <v>2187.3869346733668</v>
+      </c>
+      <c r="P59">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A60" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" s="6">
+        <v>12</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E60" s="7">
+        <v>0</v>
+      </c>
+      <c r="F60" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="G54" s="8">
+      <c r="G60" s="8">
         <v>0</v>
       </c>
-      <c r="H54" s="15">
-        <v>0.22358339951050801</v>
-      </c>
-      <c r="I54" s="15">
-        <v>0.31949703331092766</v>
-      </c>
-      <c r="J54" s="15">
-        <v>0.63491193064385332</v>
-      </c>
-      <c r="K54" s="15">
-        <v>0.9375577101334901</v>
-      </c>
-      <c r="L54" s="15">
-        <v>0.97410363869288885</v>
-      </c>
-      <c r="M54" s="12">
-        <v>5</v>
-      </c>
-      <c r="N54" s="14">
-        <v>43151</v>
-      </c>
-      <c r="O54" s="12">
-        <v>1829.3480996727917</v>
-      </c>
-      <c r="P54">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A55" s="10">
-        <v>124</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C55" s="6">
-        <v>4</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E55" s="7">
-        <v>0</v>
-      </c>
-      <c r="F55" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G55" s="8">
-        <v>12</v>
-      </c>
-      <c r="H55" s="15">
-        <v>0.22717879178441977</v>
-      </c>
-      <c r="I55" s="15">
-        <v>0.20244056777673425</v>
-      </c>
-      <c r="J55" s="15">
-        <v>0.25746916611770676</v>
-      </c>
-      <c r="K55" s="15">
-        <v>0.28910792035817395</v>
-      </c>
-      <c r="L55" s="15">
-        <v>0.43806356081658154</v>
-      </c>
-      <c r="M55" s="12">
-        <v>6</v>
-      </c>
-      <c r="N55" s="14">
-        <v>43151</v>
-      </c>
-      <c r="O55" s="12">
-        <v>2333.99209486166</v>
-      </c>
-      <c r="P55">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A56" s="10">
-        <v>125</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C56" s="6">
-        <v>4</v>
-      </c>
-      <c r="D56" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E56" s="7">
-        <v>0</v>
-      </c>
-      <c r="F56" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G56" s="8">
-        <v>0</v>
-      </c>
-      <c r="H56" s="15">
-        <v>9.335457974021566E-2</v>
-      </c>
-      <c r="I56" s="15">
-        <v>0.10825248072024335</v>
-      </c>
-      <c r="J56" s="15">
-        <v>9.1898124600874806E-2</v>
-      </c>
-      <c r="K56" s="15">
-        <v>9.8328274279023242E-2</v>
-      </c>
-      <c r="L56" s="15">
-        <v>0.12613640401722154</v>
-      </c>
-      <c r="M56" s="12">
-        <v>7</v>
-      </c>
-      <c r="N56" s="14">
-        <v>43151</v>
-      </c>
-      <c r="O56" s="12">
-        <v>1990.7793578212149</v>
-      </c>
-      <c r="P56">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A57" s="10">
-        <v>126</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C57" s="6">
-        <v>1</v>
-      </c>
-      <c r="D57" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E57" s="7">
-        <v>3</v>
-      </c>
-      <c r="F57" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G57" s="8">
-        <v>0</v>
-      </c>
-      <c r="H57" s="15">
-        <v>0.18068926339384092</v>
-      </c>
-      <c r="I57" s="15">
-        <v>0.27632489613701899</v>
-      </c>
-      <c r="J57" s="15">
-        <v>0.70273394092228292</v>
-      </c>
-      <c r="K57" s="15">
-        <v>1</v>
-      </c>
-      <c r="L57" s="15">
-        <v>1</v>
-      </c>
-      <c r="M57" s="12">
-        <v>9</v>
-      </c>
-      <c r="N57" s="14">
-        <v>43151</v>
-      </c>
-      <c r="O57" s="12">
-        <v>2232.9357522301293</v>
-      </c>
-      <c r="P57">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A58" s="10">
-        <v>61</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C58" s="6">
-        <v>3</v>
-      </c>
-      <c r="D58" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E58" s="7">
-        <v>1</v>
-      </c>
-      <c r="F58" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G58" s="8">
-        <v>12</v>
-      </c>
-      <c r="H58" s="15">
-        <v>0.48847059899398787</v>
-      </c>
-      <c r="I58" s="15">
-        <v>0.93205302876170337</v>
-      </c>
-      <c r="J58" s="15">
-        <v>0.99813369003560004</v>
-      </c>
-      <c r="K58" s="15">
-        <v>0.995350440053552</v>
-      </c>
-      <c r="L58" s="15">
-        <v>0.99953671547277778</v>
-      </c>
-      <c r="M58" s="12">
-        <v>10</v>
-      </c>
-      <c r="N58" s="14">
-        <v>43151</v>
-      </c>
-      <c r="O58" s="12">
-        <v>2271.047227926078</v>
-      </c>
-      <c r="P58">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A59" s="10">
-        <v>62</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C59" s="6">
-        <v>2</v>
-      </c>
-      <c r="D59" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E59" s="7">
-        <v>2</v>
-      </c>
-      <c r="F59" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G59" s="8">
-        <v>12</v>
-      </c>
-      <c r="H59" s="15">
-        <v>0.41542222960626685</v>
-      </c>
-      <c r="I59" s="15">
-        <v>0.71151262154585393</v>
-      </c>
-      <c r="J59" s="15">
-        <v>0.99753350059226131</v>
-      </c>
-      <c r="K59" s="15">
-        <v>1</v>
-      </c>
-      <c r="L59" s="15">
-        <v>1</v>
-      </c>
-      <c r="M59" s="12">
-        <v>11</v>
-      </c>
-      <c r="N59" s="14">
-        <v>43151</v>
-      </c>
-      <c r="O59" s="12">
-        <v>2552.3503737520696</v>
-      </c>
-      <c r="P59">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A60" s="10">
-        <v>63</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C60" s="6">
-        <v>1</v>
-      </c>
-      <c r="D60" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E60" s="7">
-        <v>3</v>
-      </c>
-      <c r="F60" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G60" s="8">
-        <v>12</v>
-      </c>
-      <c r="H60" s="15">
-        <v>0.25439508455086418</v>
-      </c>
-      <c r="I60" s="15">
-        <v>0.54680623436592934</v>
-      </c>
-      <c r="J60" s="15">
-        <v>0.94983288251657516</v>
-      </c>
-      <c r="K60" s="15">
-        <v>1</v>
-      </c>
-      <c r="L60" s="15">
-        <v>1</v>
-      </c>
-      <c r="M60" s="12">
-        <v>12</v>
+      <c r="H60" s="16">
+        <v>0.23431614457893668</v>
+      </c>
+      <c r="I60" s="16">
+        <v>0.23108882558698798</v>
+      </c>
+      <c r="J60" s="16">
+        <v>0.27517452636994272</v>
+      </c>
+      <c r="K60" s="16">
+        <v>0.30234761161988</v>
+      </c>
+      <c r="L60" s="16">
+        <v>0.35836876414979529</v>
+      </c>
+      <c r="M60" s="11">
+        <v>13</v>
       </c>
       <c r="N60" s="14">
-        <v>43151</v>
+        <v>43125</v>
       </c>
       <c r="O60" s="12">
-        <v>1868.8214643931797</v>
+        <v>2336.4250000000002</v>
       </c>
       <c r="P60">
         <v>0.01</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A61" s="10">
-        <v>64</v>
+      <c r="A61" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>5</v>
@@ -3758,7 +3762,7 @@
         <v>3</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="E61" s="7">
         <v>1</v>
@@ -3769,29 +3773,29 @@
       <c r="G61" s="8">
         <v>12</v>
       </c>
-      <c r="H61" s="15">
-        <v>0.42896103463403357</v>
-      </c>
-      <c r="I61" s="15">
-        <v>0.82130655029849109</v>
-      </c>
-      <c r="J61" s="15">
-        <v>0.95553190654897913</v>
-      </c>
-      <c r="K61" s="15">
-        <v>0.94900734808188414</v>
-      </c>
-      <c r="L61" s="15">
-        <v>0.96642058433149725</v>
-      </c>
-      <c r="M61" s="12">
-        <v>13</v>
+      <c r="H61" s="16">
+        <v>0.28286912427393568</v>
+      </c>
+      <c r="I61" s="16">
+        <v>0.5932863446941754</v>
+      </c>
+      <c r="J61" s="16">
+        <v>0.95667025928959537</v>
+      </c>
+      <c r="K61" s="16">
+        <v>0.95896394745104319</v>
+      </c>
+      <c r="L61" s="16">
+        <v>0.9620820982579561</v>
+      </c>
+      <c r="M61" s="11">
+        <v>14</v>
       </c>
       <c r="N61" s="14">
-        <v>43151</v>
+        <v>43125</v>
       </c>
       <c r="O61" s="12">
-        <v>2548.2590564236548</v>
+        <v>2048.0750000000003</v>
       </c>
       <c r="P61">
         <v>0.01</v>
@@ -4053,6 +4057,9 @@
       <c r="H141" s="13"/>
     </row>
   </sheetData>
+  <sortState ref="A2:P141">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>